<commit_message>
More Pixels and Stuff
</commit_message>
<xml_diff>
--- a/data/CTRPG Spreadsheet.xlsx
+++ b/data/CTRPG Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djerr\Documents\Game Development\Projects\Crafting RPG Tactics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8339EB-81A6-44A0-8E3A-0D2F1671CD15}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A96F0-B10B-4D83-AABD-80D40B70BD18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F75CB246-C95A-43CB-8149-AE7C498DED0C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="4" xr2:uid="{F75CB246-C95A-43CB-8149-AE7C498DED0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="2" r:id="rId1"/>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED3B433-3643-4E44-867E-7CA1D3769DAA}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1692,11 +1692,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H13" xr:uid="{6CC5B39F-8091-42C0-B493-24435249D556}">
-    <sortState ref="A2:H13">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
       <sortCondition ref="A1:A13"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:H13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1909,7 +1909,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2072,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E80F3B-D207-4DC3-993A-57489E558763}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>